<commit_message>
using customer format on date
</commit_message>
<xml_diff>
--- a/第1章 学习做表/1.2.1 把Excel当笔记本用.xlsx
+++ b/第1章 学习做表/1.2.1 把Excel当笔记本用.xlsx
@@ -13,7 +13,7 @@
     <sheet name="销售部" sheetId="4" r:id="rId4"/>
     <sheet name="统计1" sheetId="5" r:id="rId5"/>
     <sheet name="统计2" sheetId="8" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="11" r:id="rId7"/>
     <sheet name="多表合并" sheetId="6" r:id="rId8"/>
     <sheet name="多表合并（优化）" sheetId="9" r:id="rId9"/>
     <sheet name="透视表" sheetId="7" r:id="rId10"/>
@@ -23,13 +23,13 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId11"/>
+    <pivotCache cacheId="3" r:id="rId11"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="40">
   <si>
     <t>日期</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -164,6 +164,12 @@
   <si>
     <t>Apr</t>
   </si>
+  <si>
+    <t>Qtr1</t>
+  </si>
+  <si>
+    <t>Qtr2</t>
+  </si>
 </sst>
 </file>
 
@@ -259,7 +265,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -290,29 +296,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="9">
     <dxf>
       <border>
         <left style="thin">
@@ -359,28 +368,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
     </dxf>
     <dxf>
       <border>
@@ -568,7 +555,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[1.2.1 把Excel当笔记本用.xlsx]Sheet1!PivotTable2</c:name>
+    <c:name>[1.2.1 把Excel当笔记本用.xlsx]Sheet1!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -603,28 +590,38 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$7</c:f>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -657,28 +654,38 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$7</c:f>
+              <c:f>Sheet1!$C$3:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -705,28 +712,38 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$7</c:f>
+              <c:f>Sheet1!$D$3:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -753,28 +770,38 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$7</c:f>
+              <c:f>Sheet1!$E$3:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -807,28 +834,38 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$7</c:f>
+              <c:f>Sheet1!$F$3:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -855,28 +892,38 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$3:$G$7</c:f>
+              <c:f>Sheet1!$G$3:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -909,28 +956,38 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$7</c:f>
+              <c:f>Sheet1!$H$3:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -960,28 +1017,38 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$3:$I$7</c:f>
+              <c:f>Sheet1!$I$3:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1011,28 +1078,38 @@
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Jan</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Feb</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Mar</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Apr</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Jan</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Feb</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Mar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Apr</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Qtr1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Qtr2</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$7</c:f>
+              <c:f>Sheet1!$J$3:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1052,11 +1129,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="121567488"/>
-        <c:axId val="130462080"/>
+        <c:axId val="122961920"/>
+        <c:axId val="122963456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="121567488"/>
+        <c:axId val="122961920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1065,7 +1142,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130462080"/>
+        <c:crossAx val="122963456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1073,7 +1150,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="130462080"/>
+        <c:axId val="122963456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1084,7 +1161,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="121567488"/>
+        <c:crossAx val="122961920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1121,15 +1198,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1157,7 +1234,7 @@
   <cacheSource type="worksheet">
     <worksheetSource ref="A3:F22" sheet="多表合并"/>
   </cacheSource>
-  <cacheFields count="6">
+  <cacheFields count="7">
     <cacheField name="日期" numFmtId="14">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2013-01-19T00:00:00" maxDate="2013-04-24T00:00:00" count="17">
         <d v="2013-01-20T00:00:00"/>
@@ -1178,7 +1255,7 @@
         <d v="2013-03-16T00:00:00"/>
         <d v="2013-04-13T00:00:00"/>
       </sharedItems>
-      <fieldGroup base="0">
+      <fieldGroup par="6" base="0">
         <rangePr groupBy="months" startDate="2013-01-19T00:00:00" endDate="2013-04-24T00:00:00"/>
         <groupItems count="14">
           <s v="&lt;01/19/2013"/>
@@ -1222,6 +1299,19 @@
     </cacheField>
     <cacheField name="部门" numFmtId="0">
       <sharedItems/>
+    </cacheField>
+    <cacheField name="Quarters" numFmtId="0" databaseField="0">
+      <fieldGroup base="0">
+        <rangePr groupBy="quarters" startDate="2013-01-19T00:00:00" endDate="2013-04-24T00:00:00"/>
+        <groupItems count="6">
+          <s v="&lt;01/19/2013"/>
+          <s v="Qtr1"/>
+          <s v="Qtr2"/>
+          <s v="Qtr3"/>
+          <s v="Qtr4"/>
+          <s v="&gt;04/24/2013"/>
+        </groupItems>
+      </fieldGroup>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -1390,9 +1480,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A1:K7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:K9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
       <items count="15">
         <item x="0"/>
@@ -1430,21 +1520,38 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
+    <field x="6"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="7">
     <i>
       <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
     </i>
     <i>
       <x v="2"/>
     </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
+    <i r="1">
       <x v="4"/>
     </i>
     <i t="grand">
@@ -1510,9 +1617,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A1:K7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="数据透视表1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="值" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A1:K9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="7">
     <pivotField axis="axisRow" numFmtId="14" showAll="0">
       <items count="15">
         <item x="0"/>
@@ -1550,21 +1657,38 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
+    <field x="6"/>
     <field x="0"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="7">
     <i>
       <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
     </i>
     <i>
       <x v="2"/>
     </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
+    <i r="1">
       <x v="4"/>
     </i>
     <i t="grand">
@@ -1610,13 +1734,13 @@
     <dataField name="求和项:数量" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="9">
+    <format dxfId="8">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="8">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="7">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -2069,7 +2193,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -2130,138 +2254,168 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B4" s="10">
         <v>3</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11">
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11">
+      <c r="F4" s="10"/>
+      <c r="G4" s="10">
         <v>5</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11">
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10">
         <v>5</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K4" s="10">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="14" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11">
+      <c r="C5" s="10"/>
+      <c r="D5" s="10">
         <v>10</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E5" s="10">
         <v>1</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11">
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10">
         <v>20</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11">
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:11">
+      <c r="A6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B6" s="10">
         <v>5</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C6" s="10">
         <v>2</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11">
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10">
         <v>2</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11">
+      <c r="G6" s="10"/>
+      <c r="H6" s="10">
         <v>10</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I6" s="10">
         <v>5</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J6" s="10">
         <v>3</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K6" s="10">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="14" t="s">
+    <row r="7" spans="1:11">
+      <c r="A7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10">
         <v>4</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10">
         <v>10</v>
       </c>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11">
+      <c r="I8" s="10"/>
+      <c r="J8" s="10">
         <v>2</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K8" s="10">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="10" t="s">
+    <row r="9" spans="1:11">
+      <c r="A9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B9" s="10">
         <v>10</v>
       </c>
-      <c r="C7" s="11">
+      <c r="C9" s="10">
         <v>6</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D9" s="10">
         <v>10</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E9" s="10">
         <v>2</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F9" s="10">
         <v>2</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G9" s="10">
         <v>5</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H9" s="10">
         <v>40</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I9" s="10">
         <v>5</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J9" s="10">
         <v>10</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K9" s="10">
         <v>90</v>
       </c>
     </row>
@@ -3126,10 +3280,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3187,138 +3341,168 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B4" s="12">
         <v>3</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15">
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12">
         <v>5</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F4" s="12">
         <v>5</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15">
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12">
         <v>1</v>
       </c>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15">
+      <c r="J4" s="12"/>
+      <c r="K4" s="12">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="14" t="s">
+    <row r="5" spans="1:11">
+      <c r="A5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B5" s="12">
         <v>2</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15">
+      <c r="C5" s="12"/>
+      <c r="D5" s="12">
         <v>10</v>
       </c>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12">
         <v>20</v>
       </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12">
         <v>1</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15">
+      <c r="J5" s="12"/>
+      <c r="K5" s="12">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="14" t="s">
+    <row r="6" spans="1:11">
+      <c r="A6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B6" s="12">
         <v>5</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C6" s="12">
         <v>5</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12">
         <v>3</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15">
+      <c r="F6" s="12"/>
+      <c r="G6" s="12">
         <v>10</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H6" s="12">
         <v>2</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15">
+      <c r="I6" s="12"/>
+      <c r="J6" s="12">
         <v>2</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K6" s="12">
         <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15">
-        <v>2</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15">
-        <v>10</v>
-      </c>
-      <c r="H6" s="15">
-        <v>4</v>
-      </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12">
+        <v>2</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12">
+        <v>10</v>
+      </c>
+      <c r="H8" s="12">
+        <v>4</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B9" s="12">
         <v>10</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C9" s="12">
         <v>5</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D9" s="12">
         <v>10</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E9" s="12">
         <v>10</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F9" s="12">
         <v>5</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G9" s="12">
         <v>40</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H9" s="12">
         <v>6</v>
       </c>
-      <c r="I7" s="15">
+      <c r="I9" s="12">
         <v>2</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J9" s="12">
         <v>2</v>
       </c>
-      <c r="K7" s="15">
+      <c r="K9" s="12">
         <v>90</v>
       </c>
     </row>
@@ -3336,10 +3520,13 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="A3:F22"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25">
       <c r="A1" s="13" t="s">
@@ -3370,7 +3557,7 @@
       <c r="F3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3803,6 +3990,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3841,7 +4029,7 @@
       <c r="F1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>